<commit_message>
created home page, navbar and imported dependencies
</commit_message>
<xml_diff>
--- a/T3-Reports/T3_query_091520.xlsx
+++ b/T3-Reports/T3_query_091520.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louie/NetBeansProjects/mthree_projects/order-book-project-team-3/T3-Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795407B0-0AF7-484B-9D49-C036B02E9B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE52D4C-BE3B-314E-98F1-6A9E0D2B3FC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23600" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{DDA712E8-6EDA-4238-8DA3-86257BCBAB72}"/>
   </bookViews>
@@ -902,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E078EC2-A1C0-4820-B2BA-09111DDDDDA4}">
   <dimension ref="A2:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" ht="112" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="70" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>7</v>
       </c>
@@ -1212,7 +1212,9 @@
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
+      <c r="J15" s="17">
+        <v>44089</v>
+      </c>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="154" customHeight="1" x14ac:dyDescent="0.2">
@@ -1237,7 +1239,9 @@
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
+      <c r="J16" s="17">
+        <v>44089</v>
+      </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="214" customHeight="1" x14ac:dyDescent="0.2">
@@ -1252,7 +1256,7 @@
         <v>31</v>
       </c>
       <c r="E17" s="17">
-        <v>44088</v>
+        <v>44089</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>38</v>

</xml_diff>